<commit_message>
Liste Standeskommission aktualisiert und ergänzt
</commit_message>
<xml_diff>
--- a/gender ratio/standeskommission.xlsx
+++ b/gender ratio/standeskommission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gender ratio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD95454-A18A-410A-8AB6-EAA6D0FFABF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAC6D46-709E-461B-ACFC-A63E8EC928B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{669C7B45-B26B-4B76-A8C9-B2BF60283C86}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="83">
   <si>
     <t>Jahr</t>
   </si>
@@ -180,6 +180,111 @@
   </si>
   <si>
     <t>Lorenz</t>
+  </si>
+  <si>
+    <t>Schmid-Sutter</t>
+  </si>
+  <si>
+    <t>Carlo</t>
+  </si>
+  <si>
+    <t>Looser</t>
+  </si>
+  <si>
+    <t>Melchior</t>
+  </si>
+  <si>
+    <t>Moser</t>
+  </si>
+  <si>
+    <t>Sepp</t>
+  </si>
+  <si>
+    <t>Ebneter</t>
+  </si>
+  <si>
+    <t>Werner</t>
+  </si>
+  <si>
+    <t>Statthalter</t>
+  </si>
+  <si>
+    <t>Koster</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Wyser</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Wild</t>
+  </si>
+  <si>
+    <t>Alfred</t>
+  </si>
+  <si>
+    <t>Hörler</t>
+  </si>
+  <si>
+    <t>Josef</t>
+  </si>
+  <si>
+    <t>Loepfe</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Metzler-Arnold</t>
+  </si>
+  <si>
+    <t>Ruth</t>
+  </si>
+  <si>
+    <t>Frau Säckelmeister</t>
+  </si>
+  <si>
+    <t>Charly</t>
+  </si>
+  <si>
+    <t>Armleutsäckelmeister</t>
+  </si>
+  <si>
+    <t>Bischofberger</t>
+  </si>
+  <si>
+    <t>Walter</t>
+  </si>
+  <si>
+    <t>Zeugherr</t>
+  </si>
+  <si>
+    <t>Baudepartement</t>
+  </si>
+  <si>
+    <t>Fürsorgedepartement</t>
+  </si>
+  <si>
+    <t>Justiz- und Polizeidepartement</t>
+  </si>
+  <si>
+    <t>Militärdepartement</t>
+  </si>
+  <si>
+    <t>Sanitätsdepartement</t>
+  </si>
+  <si>
+    <t>Fürsorgedepartement &amp; Sanitätsdepartement</t>
+  </si>
+  <si>
+    <t>Landwirtschaftsdepartement</t>
+  </si>
+  <si>
+    <t>Justiz- und Polizeidepartement &amp; Militärdepartement</t>
   </si>
 </sst>
 </file>
@@ -551,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB2D094-259F-4BDA-9CCC-AC85399FAC35}">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E224" sqref="E224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +669,7 @@
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -592,19 +697,19 @@
         <v>2025</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -612,19 +717,19 @@
         <v>2025</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -732,7 +837,7 @@
         <v>2024</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -741,10 +846,10 @@
         <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -752,7 +857,7 @@
         <v>2024</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -761,10 +866,10 @@
         <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -872,7 +977,7 @@
         <v>2023</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
@@ -881,10 +986,10 @@
         <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -892,7 +997,7 @@
         <v>2023</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
@@ -901,10 +1006,10 @@
         <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -941,7 +1046,7 @@
         <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -1012,7 +1117,7 @@
         <v>2022</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
         <v>28</v>
@@ -1021,10 +1126,10 @@
         <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,7 +1137,7 @@
         <v>2022</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
@@ -1041,10 +1146,10 @@
         <v>35</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F24" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1081,7 +1186,7 @@
         <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
         <v>14</v>
@@ -1152,7 +1257,7 @@
         <v>2021</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
         <v>28</v>
@@ -1161,10 +1266,10 @@
         <v>35</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1172,7 +1277,7 @@
         <v>2021</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
@@ -1181,10 +1286,10 @@
         <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F31" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1221,7 +1326,7 @@
         <v>35</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F33" t="s">
         <v>14</v>
@@ -1292,7 +1397,7 @@
         <v>2020</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
         <v>28</v>
@@ -1301,10 +1406,10 @@
         <v>35</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F37" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1312,7 +1417,7 @@
         <v>2020</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
         <v>28</v>
@@ -1321,10 +1426,10 @@
         <v>35</v>
       </c>
       <c r="E38" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1361,7 +1466,7 @@
         <v>35</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F40" t="s">
         <v>14</v>
@@ -1432,7 +1537,7 @@
         <v>2019</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
         <v>28</v>
@@ -1441,10 +1546,10 @@
         <v>35</v>
       </c>
       <c r="E44" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F44" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1452,7 +1557,7 @@
         <v>2019</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C45" t="s">
         <v>28</v>
@@ -1461,10 +1566,10 @@
         <v>35</v>
       </c>
       <c r="E45" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F45" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1501,7 +1606,7 @@
         <v>35</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F47" t="s">
         <v>14</v>
@@ -1572,19 +1677,19 @@
         <v>2018</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D51" t="s">
         <v>35</v>
       </c>
       <c r="E51" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F51" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,19 +1697,19 @@
         <v>2018</v>
       </c>
       <c r="B52" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C52" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D52" t="s">
         <v>35</v>
       </c>
       <c r="E52" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F52" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1641,7 +1746,7 @@
         <v>35</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F54" t="s">
         <v>14</v>
@@ -1712,19 +1817,19 @@
         <v>2017</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C58" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D58" t="s">
         <v>35</v>
       </c>
       <c r="E58" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F58" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1732,19 +1837,19 @@
         <v>2017</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D59" t="s">
         <v>35</v>
       </c>
       <c r="E59" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1781,7 +1886,7 @@
         <v>35</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F61" t="s">
         <v>14</v>
@@ -1852,19 +1957,19 @@
         <v>2016</v>
       </c>
       <c r="B65" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D65" t="s">
         <v>35</v>
       </c>
       <c r="E65" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F65" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1872,19 +1977,19 @@
         <v>2016</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C66" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D66" t="s">
         <v>35</v>
       </c>
       <c r="E66" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F66" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1921,7 +2026,7 @@
         <v>35</v>
       </c>
       <c r="E68" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F68" t="s">
         <v>14</v>
@@ -1992,19 +2097,19 @@
         <v>2015</v>
       </c>
       <c r="B72" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C72" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D72" t="s">
         <v>35</v>
       </c>
       <c r="E72" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F72" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,19 +2117,19 @@
         <v>2015</v>
       </c>
       <c r="B73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C73" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D73" t="s">
         <v>35</v>
       </c>
       <c r="E73" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F73" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2061,7 +2166,7 @@
         <v>35</v>
       </c>
       <c r="E75" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F75" t="s">
         <v>14</v>
@@ -2132,19 +2237,19 @@
         <v>2014</v>
       </c>
       <c r="B79" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C79" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D79" t="s">
         <v>35</v>
       </c>
       <c r="E79" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F79" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2152,19 +2257,19 @@
         <v>2014</v>
       </c>
       <c r="B80" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C80" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D80" t="s">
         <v>35</v>
       </c>
       <c r="E80" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="F80" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2201,7 +2306,7 @@
         <v>35</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F82" t="s">
         <v>14</v>
@@ -2265,6 +2370,2786 @@
       </c>
       <c r="F85" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2013</v>
+      </c>
+      <c r="B86" t="s">
+        <v>39</v>
+      </c>
+      <c r="C86" t="s">
+        <v>41</v>
+      </c>
+      <c r="D86" t="s">
+        <v>35</v>
+      </c>
+      <c r="E86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2013</v>
+      </c>
+      <c r="B87" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" t="s">
+        <v>28</v>
+      </c>
+      <c r="D87" t="s">
+        <v>35</v>
+      </c>
+      <c r="E87" t="s">
+        <v>37</v>
+      </c>
+      <c r="F87" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>2013</v>
+      </c>
+      <c r="B88" t="s">
+        <v>39</v>
+      </c>
+      <c r="C88" t="s">
+        <v>40</v>
+      </c>
+      <c r="D88" t="s">
+        <v>3</v>
+      </c>
+      <c r="E88" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>2013</v>
+      </c>
+      <c r="B89" t="s">
+        <v>44</v>
+      </c>
+      <c r="C89" t="s">
+        <v>45</v>
+      </c>
+      <c r="D89" t="s">
+        <v>35</v>
+      </c>
+      <c r="E89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2013</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>47</v>
+      </c>
+      <c r="D90" t="s">
+        <v>35</v>
+      </c>
+      <c r="E90" t="s">
+        <v>15</v>
+      </c>
+      <c r="F90" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>2013</v>
+      </c>
+      <c r="B91" t="s">
+        <v>46</v>
+      </c>
+      <c r="C91" t="s">
+        <v>31</v>
+      </c>
+      <c r="D91" t="s">
+        <v>35</v>
+      </c>
+      <c r="E91" t="s">
+        <v>17</v>
+      </c>
+      <c r="F91" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>2013</v>
+      </c>
+      <c r="B92" t="s">
+        <v>42</v>
+      </c>
+      <c r="C92" t="s">
+        <v>43</v>
+      </c>
+      <c r="D92" t="s">
+        <v>35</v>
+      </c>
+      <c r="E92" t="s">
+        <v>19</v>
+      </c>
+      <c r="F92" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>2012</v>
+      </c>
+      <c r="B93" t="s">
+        <v>39</v>
+      </c>
+      <c r="C93" t="s">
+        <v>41</v>
+      </c>
+      <c r="D93" t="s">
+        <v>35</v>
+      </c>
+      <c r="E93" t="s">
+        <v>37</v>
+      </c>
+      <c r="F93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>2012</v>
+      </c>
+      <c r="B94" t="s">
+        <v>48</v>
+      </c>
+      <c r="C94" t="s">
+        <v>49</v>
+      </c>
+      <c r="D94" t="s">
+        <v>35</v>
+      </c>
+      <c r="E94" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2012</v>
+      </c>
+      <c r="B95" t="s">
+        <v>39</v>
+      </c>
+      <c r="C95" t="s">
+        <v>40</v>
+      </c>
+      <c r="D95" t="s">
+        <v>3</v>
+      </c>
+      <c r="E95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>2012</v>
+      </c>
+      <c r="B96" t="s">
+        <v>44</v>
+      </c>
+      <c r="C96" t="s">
+        <v>45</v>
+      </c>
+      <c r="D96" t="s">
+        <v>35</v>
+      </c>
+      <c r="E96" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>2012</v>
+      </c>
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>47</v>
+      </c>
+      <c r="D97" t="s">
+        <v>35</v>
+      </c>
+      <c r="E97" t="s">
+        <v>15</v>
+      </c>
+      <c r="F97" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>2012</v>
+      </c>
+      <c r="B98" t="s">
+        <v>46</v>
+      </c>
+      <c r="C98" t="s">
+        <v>31</v>
+      </c>
+      <c r="D98" t="s">
+        <v>35</v>
+      </c>
+      <c r="E98" t="s">
+        <v>17</v>
+      </c>
+      <c r="F98" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>2012</v>
+      </c>
+      <c r="B99" t="s">
+        <v>42</v>
+      </c>
+      <c r="C99" t="s">
+        <v>43</v>
+      </c>
+      <c r="D99" t="s">
+        <v>35</v>
+      </c>
+      <c r="E99" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>2011</v>
+      </c>
+      <c r="B100" t="s">
+        <v>39</v>
+      </c>
+      <c r="C100" t="s">
+        <v>41</v>
+      </c>
+      <c r="D100" t="s">
+        <v>35</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>2011</v>
+      </c>
+      <c r="B101" t="s">
+        <v>48</v>
+      </c>
+      <c r="C101" t="s">
+        <v>49</v>
+      </c>
+      <c r="D101" t="s">
+        <v>35</v>
+      </c>
+      <c r="E101" t="s">
+        <v>37</v>
+      </c>
+      <c r="F101" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2011</v>
+      </c>
+      <c r="B102" t="s">
+        <v>39</v>
+      </c>
+      <c r="C102" t="s">
+        <v>40</v>
+      </c>
+      <c r="D102" t="s">
+        <v>3</v>
+      </c>
+      <c r="E102" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>2011</v>
+      </c>
+      <c r="B103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C103" t="s">
+        <v>45</v>
+      </c>
+      <c r="D103" t="s">
+        <v>35</v>
+      </c>
+      <c r="E103" t="s">
+        <v>13</v>
+      </c>
+      <c r="F103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>2011</v>
+      </c>
+      <c r="B104" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" t="s">
+        <v>47</v>
+      </c>
+      <c r="D104" t="s">
+        <v>35</v>
+      </c>
+      <c r="E104" t="s">
+        <v>15</v>
+      </c>
+      <c r="F104" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>2011</v>
+      </c>
+      <c r="B105" t="s">
+        <v>46</v>
+      </c>
+      <c r="C105" t="s">
+        <v>31</v>
+      </c>
+      <c r="D105" t="s">
+        <v>35</v>
+      </c>
+      <c r="E105" t="s">
+        <v>17</v>
+      </c>
+      <c r="F105" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>2011</v>
+      </c>
+      <c r="B106" t="s">
+        <v>50</v>
+      </c>
+      <c r="C106" t="s">
+        <v>51</v>
+      </c>
+      <c r="D106" t="s">
+        <v>35</v>
+      </c>
+      <c r="E106" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>2010</v>
+      </c>
+      <c r="B107" t="s">
+        <v>39</v>
+      </c>
+      <c r="C107" t="s">
+        <v>41</v>
+      </c>
+      <c r="D107" t="s">
+        <v>35</v>
+      </c>
+      <c r="E107" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2010</v>
+      </c>
+      <c r="B108" t="s">
+        <v>48</v>
+      </c>
+      <c r="C108" t="s">
+        <v>49</v>
+      </c>
+      <c r="D108" t="s">
+        <v>35</v>
+      </c>
+      <c r="E108" t="s">
+        <v>37</v>
+      </c>
+      <c r="F108" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2010</v>
+      </c>
+      <c r="B109" t="s">
+        <v>39</v>
+      </c>
+      <c r="C109" t="s">
+        <v>40</v>
+      </c>
+      <c r="D109" t="s">
+        <v>3</v>
+      </c>
+      <c r="E109" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>2010</v>
+      </c>
+      <c r="B110" t="s">
+        <v>52</v>
+      </c>
+      <c r="C110" t="s">
+        <v>53</v>
+      </c>
+      <c r="D110" t="s">
+        <v>35</v>
+      </c>
+      <c r="E110" t="s">
+        <v>13</v>
+      </c>
+      <c r="F110" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>2010</v>
+      </c>
+      <c r="B111" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" t="s">
+        <v>47</v>
+      </c>
+      <c r="D111" t="s">
+        <v>35</v>
+      </c>
+      <c r="E111" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>2010</v>
+      </c>
+      <c r="B112" t="s">
+        <v>46</v>
+      </c>
+      <c r="C112" t="s">
+        <v>31</v>
+      </c>
+      <c r="D112" t="s">
+        <v>35</v>
+      </c>
+      <c r="E112" t="s">
+        <v>17</v>
+      </c>
+      <c r="F112" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>2010</v>
+      </c>
+      <c r="B113" t="s">
+        <v>50</v>
+      </c>
+      <c r="C113" t="s">
+        <v>51</v>
+      </c>
+      <c r="D113" t="s">
+        <v>35</v>
+      </c>
+      <c r="E113" t="s">
+        <v>19</v>
+      </c>
+      <c r="F113" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>2009</v>
+      </c>
+      <c r="B114" t="s">
+        <v>39</v>
+      </c>
+      <c r="C114" t="s">
+        <v>41</v>
+      </c>
+      <c r="D114" t="s">
+        <v>35</v>
+      </c>
+      <c r="E114" t="s">
+        <v>37</v>
+      </c>
+      <c r="F114" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>2009</v>
+      </c>
+      <c r="B115" t="s">
+        <v>48</v>
+      </c>
+      <c r="C115" t="s">
+        <v>49</v>
+      </c>
+      <c r="D115" t="s">
+        <v>35</v>
+      </c>
+      <c r="E115" t="s">
+        <v>9</v>
+      </c>
+      <c r="F115" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>2009</v>
+      </c>
+      <c r="B116" t="s">
+        <v>54</v>
+      </c>
+      <c r="C116" t="s">
+        <v>55</v>
+      </c>
+      <c r="D116" t="s">
+        <v>35</v>
+      </c>
+      <c r="E116" t="s">
+        <v>56</v>
+      </c>
+      <c r="F116" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>2009</v>
+      </c>
+      <c r="B117" t="s">
+        <v>52</v>
+      </c>
+      <c r="C117" t="s">
+        <v>53</v>
+      </c>
+      <c r="D117" t="s">
+        <v>35</v>
+      </c>
+      <c r="E117" t="s">
+        <v>13</v>
+      </c>
+      <c r="F117" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>2009</v>
+      </c>
+      <c r="B118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" t="s">
+        <v>47</v>
+      </c>
+      <c r="D118" t="s">
+        <v>35</v>
+      </c>
+      <c r="E118" t="s">
+        <v>15</v>
+      </c>
+      <c r="F118" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>2009</v>
+      </c>
+      <c r="B119" t="s">
+        <v>46</v>
+      </c>
+      <c r="C119" t="s">
+        <v>31</v>
+      </c>
+      <c r="D119" t="s">
+        <v>35</v>
+      </c>
+      <c r="E119" t="s">
+        <v>17</v>
+      </c>
+      <c r="F119" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>2009</v>
+      </c>
+      <c r="B120" t="s">
+        <v>50</v>
+      </c>
+      <c r="C120" t="s">
+        <v>51</v>
+      </c>
+      <c r="D120" t="s">
+        <v>35</v>
+      </c>
+      <c r="E120" t="s">
+        <v>19</v>
+      </c>
+      <c r="F120" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>2008</v>
+      </c>
+      <c r="B121" t="s">
+        <v>39</v>
+      </c>
+      <c r="C121" t="s">
+        <v>41</v>
+      </c>
+      <c r="D121" t="s">
+        <v>35</v>
+      </c>
+      <c r="E121" t="s">
+        <v>37</v>
+      </c>
+      <c r="F121" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>2008</v>
+      </c>
+      <c r="B122" t="s">
+        <v>48</v>
+      </c>
+      <c r="C122" t="s">
+        <v>49</v>
+      </c>
+      <c r="D122" t="s">
+        <v>35</v>
+      </c>
+      <c r="E122" t="s">
+        <v>9</v>
+      </c>
+      <c r="F122" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>2008</v>
+      </c>
+      <c r="B123" t="s">
+        <v>54</v>
+      </c>
+      <c r="C123" t="s">
+        <v>55</v>
+      </c>
+      <c r="D123" t="s">
+        <v>35</v>
+      </c>
+      <c r="E123" t="s">
+        <v>56</v>
+      </c>
+      <c r="F123" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>2008</v>
+      </c>
+      <c r="B124" t="s">
+        <v>52</v>
+      </c>
+      <c r="C124" t="s">
+        <v>53</v>
+      </c>
+      <c r="D124" t="s">
+        <v>35</v>
+      </c>
+      <c r="E124" t="s">
+        <v>13</v>
+      </c>
+      <c r="F124" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>2008</v>
+      </c>
+      <c r="B125" t="s">
+        <v>8</v>
+      </c>
+      <c r="C125" t="s">
+        <v>47</v>
+      </c>
+      <c r="D125" t="s">
+        <v>35</v>
+      </c>
+      <c r="E125" t="s">
+        <v>15</v>
+      </c>
+      <c r="F125" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>2008</v>
+      </c>
+      <c r="B126" t="s">
+        <v>46</v>
+      </c>
+      <c r="C126" t="s">
+        <v>31</v>
+      </c>
+      <c r="D126" t="s">
+        <v>35</v>
+      </c>
+      <c r="E126" t="s">
+        <v>17</v>
+      </c>
+      <c r="F126" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>2008</v>
+      </c>
+      <c r="B127" t="s">
+        <v>50</v>
+      </c>
+      <c r="C127" t="s">
+        <v>51</v>
+      </c>
+      <c r="D127" t="s">
+        <v>35</v>
+      </c>
+      <c r="E127" t="s">
+        <v>19</v>
+      </c>
+      <c r="F127" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>2007</v>
+      </c>
+      <c r="B128" t="s">
+        <v>57</v>
+      </c>
+      <c r="C128" t="s">
+        <v>58</v>
+      </c>
+      <c r="D128" t="s">
+        <v>35</v>
+      </c>
+      <c r="E128" t="s">
+        <v>9</v>
+      </c>
+      <c r="F128" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>2007</v>
+      </c>
+      <c r="B129" t="s">
+        <v>48</v>
+      </c>
+      <c r="C129" t="s">
+        <v>49</v>
+      </c>
+      <c r="D129" t="s">
+        <v>35</v>
+      </c>
+      <c r="E129" t="s">
+        <v>37</v>
+      </c>
+      <c r="F129" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>2007</v>
+      </c>
+      <c r="B130" t="s">
+        <v>54</v>
+      </c>
+      <c r="C130" t="s">
+        <v>55</v>
+      </c>
+      <c r="D130" t="s">
+        <v>35</v>
+      </c>
+      <c r="E130" t="s">
+        <v>56</v>
+      </c>
+      <c r="F130" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>2007</v>
+      </c>
+      <c r="B131" t="s">
+        <v>52</v>
+      </c>
+      <c r="C131" t="s">
+        <v>53</v>
+      </c>
+      <c r="D131" t="s">
+        <v>35</v>
+      </c>
+      <c r="E131" t="s">
+        <v>13</v>
+      </c>
+      <c r="F131" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>2007</v>
+      </c>
+      <c r="B132" t="s">
+        <v>8</v>
+      </c>
+      <c r="C132" t="s">
+        <v>47</v>
+      </c>
+      <c r="D132" t="s">
+        <v>35</v>
+      </c>
+      <c r="E132" t="s">
+        <v>15</v>
+      </c>
+      <c r="F132" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>2007</v>
+      </c>
+      <c r="B133" t="s">
+        <v>46</v>
+      </c>
+      <c r="C133" t="s">
+        <v>31</v>
+      </c>
+      <c r="D133" t="s">
+        <v>35</v>
+      </c>
+      <c r="E133" t="s">
+        <v>17</v>
+      </c>
+      <c r="F133" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>2007</v>
+      </c>
+      <c r="B134" t="s">
+        <v>50</v>
+      </c>
+      <c r="C134" t="s">
+        <v>51</v>
+      </c>
+      <c r="D134" t="s">
+        <v>35</v>
+      </c>
+      <c r="E134" t="s">
+        <v>19</v>
+      </c>
+      <c r="F134" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>2006</v>
+      </c>
+      <c r="B135" t="s">
+        <v>57</v>
+      </c>
+      <c r="C135" t="s">
+        <v>58</v>
+      </c>
+      <c r="D135" t="s">
+        <v>35</v>
+      </c>
+      <c r="E135" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>2006</v>
+      </c>
+      <c r="B136" t="s">
+        <v>48</v>
+      </c>
+      <c r="C136" t="s">
+        <v>49</v>
+      </c>
+      <c r="D136" t="s">
+        <v>35</v>
+      </c>
+      <c r="E136" t="s">
+        <v>37</v>
+      </c>
+      <c r="F136" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>2006</v>
+      </c>
+      <c r="B137" t="s">
+        <v>54</v>
+      </c>
+      <c r="C137" t="s">
+        <v>55</v>
+      </c>
+      <c r="D137" t="s">
+        <v>35</v>
+      </c>
+      <c r="E137" t="s">
+        <v>56</v>
+      </c>
+      <c r="F137" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>2006</v>
+      </c>
+      <c r="B138" t="s">
+        <v>59</v>
+      </c>
+      <c r="C138" t="s">
+        <v>60</v>
+      </c>
+      <c r="D138" t="s">
+        <v>35</v>
+      </c>
+      <c r="E138" t="s">
+        <v>13</v>
+      </c>
+      <c r="F138" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>2006</v>
+      </c>
+      <c r="B139" t="s">
+        <v>8</v>
+      </c>
+      <c r="C139" t="s">
+        <v>47</v>
+      </c>
+      <c r="D139" t="s">
+        <v>35</v>
+      </c>
+      <c r="E139" t="s">
+        <v>15</v>
+      </c>
+      <c r="F139" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>2006</v>
+      </c>
+      <c r="B140" t="s">
+        <v>46</v>
+      </c>
+      <c r="C140" t="s">
+        <v>31</v>
+      </c>
+      <c r="D140" t="s">
+        <v>35</v>
+      </c>
+      <c r="E140" t="s">
+        <v>17</v>
+      </c>
+      <c r="F140" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>2006</v>
+      </c>
+      <c r="B141" t="s">
+        <v>50</v>
+      </c>
+      <c r="C141" t="s">
+        <v>51</v>
+      </c>
+      <c r="D141" t="s">
+        <v>35</v>
+      </c>
+      <c r="E141" t="s">
+        <v>19</v>
+      </c>
+      <c r="F141" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>2005</v>
+      </c>
+      <c r="B142" t="s">
+        <v>57</v>
+      </c>
+      <c r="C142" t="s">
+        <v>58</v>
+      </c>
+      <c r="D142" t="s">
+        <v>35</v>
+      </c>
+      <c r="E142" t="s">
+        <v>37</v>
+      </c>
+      <c r="F142" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>2005</v>
+      </c>
+      <c r="B143" t="s">
+        <v>48</v>
+      </c>
+      <c r="C143" t="s">
+        <v>49</v>
+      </c>
+      <c r="D143" t="s">
+        <v>35</v>
+      </c>
+      <c r="E143" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>2005</v>
+      </c>
+      <c r="B144" t="s">
+        <v>54</v>
+      </c>
+      <c r="C144" t="s">
+        <v>55</v>
+      </c>
+      <c r="D144" t="s">
+        <v>35</v>
+      </c>
+      <c r="E144" t="s">
+        <v>56</v>
+      </c>
+      <c r="F144" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>2005</v>
+      </c>
+      <c r="B145" t="s">
+        <v>59</v>
+      </c>
+      <c r="C145" t="s">
+        <v>60</v>
+      </c>
+      <c r="D145" t="s">
+        <v>35</v>
+      </c>
+      <c r="E145" t="s">
+        <v>13</v>
+      </c>
+      <c r="F145" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>2005</v>
+      </c>
+      <c r="B146" t="s">
+        <v>8</v>
+      </c>
+      <c r="C146" t="s">
+        <v>47</v>
+      </c>
+      <c r="D146" t="s">
+        <v>35</v>
+      </c>
+      <c r="E146" t="s">
+        <v>15</v>
+      </c>
+      <c r="F146" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>2005</v>
+      </c>
+      <c r="B147" t="s">
+        <v>46</v>
+      </c>
+      <c r="C147" t="s">
+        <v>31</v>
+      </c>
+      <c r="D147" t="s">
+        <v>35</v>
+      </c>
+      <c r="E147" t="s">
+        <v>17</v>
+      </c>
+      <c r="F147" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>2005</v>
+      </c>
+      <c r="B148" t="s">
+        <v>50</v>
+      </c>
+      <c r="C148" t="s">
+        <v>51</v>
+      </c>
+      <c r="D148" t="s">
+        <v>35</v>
+      </c>
+      <c r="E148" t="s">
+        <v>19</v>
+      </c>
+      <c r="F148" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>2003</v>
+      </c>
+      <c r="B149" t="s">
+        <v>57</v>
+      </c>
+      <c r="C149" t="s">
+        <v>58</v>
+      </c>
+      <c r="D149" t="s">
+        <v>35</v>
+      </c>
+      <c r="E149" t="s">
+        <v>9</v>
+      </c>
+      <c r="F149" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>2003</v>
+      </c>
+      <c r="B150" t="s">
+        <v>48</v>
+      </c>
+      <c r="C150" t="s">
+        <v>49</v>
+      </c>
+      <c r="D150" t="s">
+        <v>35</v>
+      </c>
+      <c r="E150" t="s">
+        <v>37</v>
+      </c>
+      <c r="F150" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>2003</v>
+      </c>
+      <c r="B151" t="s">
+        <v>54</v>
+      </c>
+      <c r="C151" t="s">
+        <v>55</v>
+      </c>
+      <c r="D151" t="s">
+        <v>35</v>
+      </c>
+      <c r="E151" t="s">
+        <v>56</v>
+      </c>
+      <c r="F151" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>2003</v>
+      </c>
+      <c r="B152" t="s">
+        <v>59</v>
+      </c>
+      <c r="C152" t="s">
+        <v>60</v>
+      </c>
+      <c r="D152" t="s">
+        <v>35</v>
+      </c>
+      <c r="E152" t="s">
+        <v>13</v>
+      </c>
+      <c r="F152" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>2003</v>
+      </c>
+      <c r="B153" t="s">
+        <v>8</v>
+      </c>
+      <c r="C153" t="s">
+        <v>47</v>
+      </c>
+      <c r="D153" t="s">
+        <v>35</v>
+      </c>
+      <c r="E153" t="s">
+        <v>15</v>
+      </c>
+      <c r="F153" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>2003</v>
+      </c>
+      <c r="B154" t="s">
+        <v>46</v>
+      </c>
+      <c r="C154" t="s">
+        <v>32</v>
+      </c>
+      <c r="D154" t="s">
+        <v>35</v>
+      </c>
+      <c r="E154" t="s">
+        <v>17</v>
+      </c>
+      <c r="F154" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>2003</v>
+      </c>
+      <c r="B155" t="s">
+        <v>61</v>
+      </c>
+      <c r="C155" t="s">
+        <v>62</v>
+      </c>
+      <c r="D155" t="s">
+        <v>35</v>
+      </c>
+      <c r="E155" t="s">
+        <v>19</v>
+      </c>
+      <c r="F155" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>2001</v>
+      </c>
+      <c r="B156" t="s">
+        <v>57</v>
+      </c>
+      <c r="C156" t="s">
+        <v>58</v>
+      </c>
+      <c r="D156" t="s">
+        <v>35</v>
+      </c>
+      <c r="E156" t="s">
+        <v>37</v>
+      </c>
+      <c r="F156" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>2001</v>
+      </c>
+      <c r="B157" t="s">
+        <v>48</v>
+      </c>
+      <c r="C157" t="s">
+        <v>49</v>
+      </c>
+      <c r="D157" t="s">
+        <v>35</v>
+      </c>
+      <c r="E157" t="s">
+        <v>9</v>
+      </c>
+      <c r="F157" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>2001</v>
+      </c>
+      <c r="B158" t="s">
+        <v>63</v>
+      </c>
+      <c r="C158" t="s">
+        <v>32</v>
+      </c>
+      <c r="D158" t="s">
+        <v>35</v>
+      </c>
+      <c r="E158" t="s">
+        <v>56</v>
+      </c>
+      <c r="F158" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>2001</v>
+      </c>
+      <c r="B159" t="s">
+        <v>59</v>
+      </c>
+      <c r="C159" t="s">
+        <v>60</v>
+      </c>
+      <c r="D159" t="s">
+        <v>35</v>
+      </c>
+      <c r="E159" t="s">
+        <v>13</v>
+      </c>
+      <c r="F159" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>2001</v>
+      </c>
+      <c r="B160" t="s">
+        <v>8</v>
+      </c>
+      <c r="C160" t="s">
+        <v>47</v>
+      </c>
+      <c r="D160" t="s">
+        <v>35</v>
+      </c>
+      <c r="E160" t="s">
+        <v>15</v>
+      </c>
+      <c r="F160" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>2001</v>
+      </c>
+      <c r="B161" t="s">
+        <v>46</v>
+      </c>
+      <c r="C161" t="s">
+        <v>32</v>
+      </c>
+      <c r="D161" t="s">
+        <v>35</v>
+      </c>
+      <c r="E161" t="s">
+        <v>17</v>
+      </c>
+      <c r="F161" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>2001</v>
+      </c>
+      <c r="B162" t="s">
+        <v>61</v>
+      </c>
+      <c r="C162" t="s">
+        <v>62</v>
+      </c>
+      <c r="D162" t="s">
+        <v>35</v>
+      </c>
+      <c r="E162" t="s">
+        <v>19</v>
+      </c>
+      <c r="F162" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>2000</v>
+      </c>
+      <c r="B163" t="s">
+        <v>57</v>
+      </c>
+      <c r="C163" t="s">
+        <v>58</v>
+      </c>
+      <c r="D163" t="s">
+        <v>35</v>
+      </c>
+      <c r="E163" t="s">
+        <v>37</v>
+      </c>
+      <c r="F163" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>2000</v>
+      </c>
+      <c r="B164" t="s">
+        <v>48</v>
+      </c>
+      <c r="C164" t="s">
+        <v>49</v>
+      </c>
+      <c r="D164" t="s">
+        <v>35</v>
+      </c>
+      <c r="E164" t="s">
+        <v>9</v>
+      </c>
+      <c r="F164" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>2000</v>
+      </c>
+      <c r="B165" t="s">
+        <v>63</v>
+      </c>
+      <c r="C165" t="s">
+        <v>32</v>
+      </c>
+      <c r="D165" t="s">
+        <v>35</v>
+      </c>
+      <c r="E165" t="s">
+        <v>56</v>
+      </c>
+      <c r="F165" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>2000</v>
+      </c>
+      <c r="B166" t="s">
+        <v>59</v>
+      </c>
+      <c r="C166" t="s">
+        <v>60</v>
+      </c>
+      <c r="D166" t="s">
+        <v>35</v>
+      </c>
+      <c r="E166" t="s">
+        <v>13</v>
+      </c>
+      <c r="F166" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>2000</v>
+      </c>
+      <c r="B167" t="s">
+        <v>36</v>
+      </c>
+      <c r="C167" t="s">
+        <v>64</v>
+      </c>
+      <c r="D167" t="s">
+        <v>35</v>
+      </c>
+      <c r="E167" t="s">
+        <v>15</v>
+      </c>
+      <c r="F167" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>2000</v>
+      </c>
+      <c r="B168" t="s">
+        <v>46</v>
+      </c>
+      <c r="C168" t="s">
+        <v>32</v>
+      </c>
+      <c r="D168" t="s">
+        <v>35</v>
+      </c>
+      <c r="E168" t="s">
+        <v>17</v>
+      </c>
+      <c r="F168" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>2000</v>
+      </c>
+      <c r="B169" t="s">
+        <v>61</v>
+      </c>
+      <c r="C169" t="s">
+        <v>62</v>
+      </c>
+      <c r="D169" t="s">
+        <v>35</v>
+      </c>
+      <c r="E169" t="s">
+        <v>19</v>
+      </c>
+      <c r="F169" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>1999</v>
+      </c>
+      <c r="B170" t="s">
+        <v>65</v>
+      </c>
+      <c r="C170" t="s">
+        <v>66</v>
+      </c>
+      <c r="D170" t="s">
+        <v>35</v>
+      </c>
+      <c r="E170" t="s">
+        <v>9</v>
+      </c>
+      <c r="F170" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>1999</v>
+      </c>
+      <c r="B171" t="s">
+        <v>48</v>
+      </c>
+      <c r="C171" t="s">
+        <v>49</v>
+      </c>
+      <c r="D171" t="s">
+        <v>35</v>
+      </c>
+      <c r="E171" t="s">
+        <v>37</v>
+      </c>
+      <c r="F171" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>1999</v>
+      </c>
+      <c r="B172" t="s">
+        <v>63</v>
+      </c>
+      <c r="C172" t="s">
+        <v>32</v>
+      </c>
+      <c r="D172" t="s">
+        <v>35</v>
+      </c>
+      <c r="E172" t="s">
+        <v>56</v>
+      </c>
+      <c r="F172" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>1999</v>
+      </c>
+      <c r="B173" t="s">
+        <v>57</v>
+      </c>
+      <c r="C173" t="s">
+        <v>58</v>
+      </c>
+      <c r="D173" t="s">
+        <v>35</v>
+      </c>
+      <c r="E173" t="s">
+        <v>13</v>
+      </c>
+      <c r="F173" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>1999</v>
+      </c>
+      <c r="B174" t="s">
+        <v>36</v>
+      </c>
+      <c r="C174" t="s">
+        <v>64</v>
+      </c>
+      <c r="D174" t="s">
+        <v>35</v>
+      </c>
+      <c r="E174" t="s">
+        <v>15</v>
+      </c>
+      <c r="F174" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>1999</v>
+      </c>
+      <c r="B175" t="s">
+        <v>46</v>
+      </c>
+      <c r="C175" t="s">
+        <v>32</v>
+      </c>
+      <c r="D175" t="s">
+        <v>35</v>
+      </c>
+      <c r="E175" t="s">
+        <v>17</v>
+      </c>
+      <c r="F175" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>1999</v>
+      </c>
+      <c r="B176" t="s">
+        <v>61</v>
+      </c>
+      <c r="C176" t="s">
+        <v>62</v>
+      </c>
+      <c r="D176" t="s">
+        <v>35</v>
+      </c>
+      <c r="E176" t="s">
+        <v>19</v>
+      </c>
+      <c r="F176" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>1998</v>
+      </c>
+      <c r="B177" t="s">
+        <v>65</v>
+      </c>
+      <c r="C177" t="s">
+        <v>66</v>
+      </c>
+      <c r="D177" t="s">
+        <v>35</v>
+      </c>
+      <c r="E177" t="s">
+        <v>9</v>
+      </c>
+      <c r="F177" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>1998</v>
+      </c>
+      <c r="B178" t="s">
+        <v>48</v>
+      </c>
+      <c r="C178" t="s">
+        <v>49</v>
+      </c>
+      <c r="D178" t="s">
+        <v>35</v>
+      </c>
+      <c r="E178" t="s">
+        <v>37</v>
+      </c>
+      <c r="F178" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>1998</v>
+      </c>
+      <c r="B179" t="s">
+        <v>63</v>
+      </c>
+      <c r="C179" t="s">
+        <v>32</v>
+      </c>
+      <c r="D179" t="s">
+        <v>35</v>
+      </c>
+      <c r="E179" t="s">
+        <v>56</v>
+      </c>
+      <c r="F179" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>1998</v>
+      </c>
+      <c r="B180" t="s">
+        <v>67</v>
+      </c>
+      <c r="C180" t="s">
+        <v>68</v>
+      </c>
+      <c r="D180" t="s">
+        <v>3</v>
+      </c>
+      <c r="E180" t="s">
+        <v>69</v>
+      </c>
+      <c r="F180" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>1998</v>
+      </c>
+      <c r="B181" t="s">
+        <v>36</v>
+      </c>
+      <c r="C181" t="s">
+        <v>64</v>
+      </c>
+      <c r="D181" t="s">
+        <v>35</v>
+      </c>
+      <c r="E181" t="s">
+        <v>15</v>
+      </c>
+      <c r="F181" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>1998</v>
+      </c>
+      <c r="B182" t="s">
+        <v>46</v>
+      </c>
+      <c r="C182" t="s">
+        <v>32</v>
+      </c>
+      <c r="D182" t="s">
+        <v>35</v>
+      </c>
+      <c r="E182" t="s">
+        <v>17</v>
+      </c>
+      <c r="F182" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>1998</v>
+      </c>
+      <c r="B183" t="s">
+        <v>61</v>
+      </c>
+      <c r="C183" t="s">
+        <v>62</v>
+      </c>
+      <c r="D183" t="s">
+        <v>35</v>
+      </c>
+      <c r="E183" t="s">
+        <v>19</v>
+      </c>
+      <c r="F183" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>1997</v>
+      </c>
+      <c r="B184" t="s">
+        <v>65</v>
+      </c>
+      <c r="C184" t="s">
+        <v>66</v>
+      </c>
+      <c r="D184" t="s">
+        <v>35</v>
+      </c>
+      <c r="E184" t="s">
+        <v>37</v>
+      </c>
+      <c r="F184" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>1997</v>
+      </c>
+      <c r="B185" t="s">
+        <v>48</v>
+      </c>
+      <c r="C185" t="s">
+        <v>49</v>
+      </c>
+      <c r="D185" t="s">
+        <v>35</v>
+      </c>
+      <c r="E185" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>1997</v>
+      </c>
+      <c r="B186" t="s">
+        <v>63</v>
+      </c>
+      <c r="C186" t="s">
+        <v>32</v>
+      </c>
+      <c r="D186" t="s">
+        <v>35</v>
+      </c>
+      <c r="E186" t="s">
+        <v>56</v>
+      </c>
+      <c r="F186" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>1997</v>
+      </c>
+      <c r="B187" t="s">
+        <v>67</v>
+      </c>
+      <c r="C187" t="s">
+        <v>68</v>
+      </c>
+      <c r="D187" t="s">
+        <v>3</v>
+      </c>
+      <c r="E187" t="s">
+        <v>69</v>
+      </c>
+      <c r="F187" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>1997</v>
+      </c>
+      <c r="B188" t="s">
+        <v>36</v>
+      </c>
+      <c r="C188" t="s">
+        <v>64</v>
+      </c>
+      <c r="D188" t="s">
+        <v>35</v>
+      </c>
+      <c r="E188" t="s">
+        <v>15</v>
+      </c>
+      <c r="F188" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>1997</v>
+      </c>
+      <c r="B189" t="s">
+        <v>46</v>
+      </c>
+      <c r="C189" t="s">
+        <v>32</v>
+      </c>
+      <c r="D189" t="s">
+        <v>35</v>
+      </c>
+      <c r="E189" t="s">
+        <v>17</v>
+      </c>
+      <c r="F189" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>1997</v>
+      </c>
+      <c r="B190" t="s">
+        <v>61</v>
+      </c>
+      <c r="C190" t="s">
+        <v>62</v>
+      </c>
+      <c r="D190" t="s">
+        <v>35</v>
+      </c>
+      <c r="E190" t="s">
+        <v>19</v>
+      </c>
+      <c r="F190" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>1996</v>
+      </c>
+      <c r="B191" t="s">
+        <v>65</v>
+      </c>
+      <c r="C191" t="s">
+        <v>66</v>
+      </c>
+      <c r="D191" t="s">
+        <v>35</v>
+      </c>
+      <c r="E191" t="s">
+        <v>37</v>
+      </c>
+      <c r="F191" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>1996</v>
+      </c>
+      <c r="B192" t="s">
+        <v>48</v>
+      </c>
+      <c r="C192" t="s">
+        <v>49</v>
+      </c>
+      <c r="D192" t="s">
+        <v>35</v>
+      </c>
+      <c r="E192" t="s">
+        <v>9</v>
+      </c>
+      <c r="F192" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>1996</v>
+      </c>
+      <c r="B193" t="s">
+        <v>63</v>
+      </c>
+      <c r="C193" t="s">
+        <v>32</v>
+      </c>
+      <c r="D193" t="s">
+        <v>35</v>
+      </c>
+      <c r="E193" t="s">
+        <v>56</v>
+      </c>
+      <c r="F193" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>1996</v>
+      </c>
+      <c r="B194" t="s">
+        <v>67</v>
+      </c>
+      <c r="C194" t="s">
+        <v>68</v>
+      </c>
+      <c r="D194" t="s">
+        <v>3</v>
+      </c>
+      <c r="E194" t="s">
+        <v>69</v>
+      </c>
+      <c r="F194" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>1996</v>
+      </c>
+      <c r="B195" t="s">
+        <v>36</v>
+      </c>
+      <c r="C195" t="s">
+        <v>64</v>
+      </c>
+      <c r="D195" t="s">
+        <v>35</v>
+      </c>
+      <c r="E195" t="s">
+        <v>15</v>
+      </c>
+      <c r="F195" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>1996</v>
+      </c>
+      <c r="B196" t="s">
+        <v>46</v>
+      </c>
+      <c r="C196" t="s">
+        <v>32</v>
+      </c>
+      <c r="D196" t="s">
+        <v>35</v>
+      </c>
+      <c r="E196" t="s">
+        <v>17</v>
+      </c>
+      <c r="F196" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>1996</v>
+      </c>
+      <c r="B197" t="s">
+        <v>61</v>
+      </c>
+      <c r="C197" t="s">
+        <v>62</v>
+      </c>
+      <c r="D197" t="s">
+        <v>35</v>
+      </c>
+      <c r="E197" t="s">
+        <v>19</v>
+      </c>
+      <c r="F197" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>1995</v>
+      </c>
+      <c r="B198" t="s">
+        <v>65</v>
+      </c>
+      <c r="C198" t="s">
+        <v>66</v>
+      </c>
+      <c r="D198" t="s">
+        <v>35</v>
+      </c>
+      <c r="E198" t="s">
+        <v>9</v>
+      </c>
+      <c r="F198" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>1995</v>
+      </c>
+      <c r="B199" t="s">
+        <v>48</v>
+      </c>
+      <c r="C199" t="s">
+        <v>49</v>
+      </c>
+      <c r="D199" t="s">
+        <v>35</v>
+      </c>
+      <c r="E199" t="s">
+        <v>37</v>
+      </c>
+      <c r="F199" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>1995</v>
+      </c>
+      <c r="B200" t="s">
+        <v>63</v>
+      </c>
+      <c r="C200" t="s">
+        <v>32</v>
+      </c>
+      <c r="D200" t="s">
+        <v>35</v>
+      </c>
+      <c r="E200" t="s">
+        <v>56</v>
+      </c>
+      <c r="F200" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>1995</v>
+      </c>
+      <c r="B201" t="s">
+        <v>39</v>
+      </c>
+      <c r="C201" t="s">
+        <v>70</v>
+      </c>
+      <c r="D201" t="s">
+        <v>35</v>
+      </c>
+      <c r="E201" t="s">
+        <v>69</v>
+      </c>
+      <c r="F201" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>1995</v>
+      </c>
+      <c r="B202" t="s">
+        <v>36</v>
+      </c>
+      <c r="C202" t="s">
+        <v>64</v>
+      </c>
+      <c r="D202" t="s">
+        <v>35</v>
+      </c>
+      <c r="E202" t="s">
+        <v>15</v>
+      </c>
+      <c r="F202" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>1995</v>
+      </c>
+      <c r="B203" t="s">
+        <v>46</v>
+      </c>
+      <c r="C203" t="s">
+        <v>32</v>
+      </c>
+      <c r="D203" t="s">
+        <v>35</v>
+      </c>
+      <c r="E203" t="s">
+        <v>17</v>
+      </c>
+      <c r="F203" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>1995</v>
+      </c>
+      <c r="B204" t="s">
+        <v>61</v>
+      </c>
+      <c r="C204" t="s">
+        <v>62</v>
+      </c>
+      <c r="D204" t="s">
+        <v>35</v>
+      </c>
+      <c r="E204" t="s">
+        <v>19</v>
+      </c>
+      <c r="F204" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>1995</v>
+      </c>
+      <c r="B205" t="s">
+        <v>46</v>
+      </c>
+      <c r="C205" t="s">
+        <v>64</v>
+      </c>
+      <c r="D205" t="s">
+        <v>35</v>
+      </c>
+      <c r="E205" t="s">
+        <v>71</v>
+      </c>
+      <c r="F205" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>1995</v>
+      </c>
+      <c r="B206" t="s">
+        <v>72</v>
+      </c>
+      <c r="C206" t="s">
+        <v>73</v>
+      </c>
+      <c r="D206" t="s">
+        <v>35</v>
+      </c>
+      <c r="E206" t="s">
+        <v>74</v>
+      </c>
+      <c r="F206" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>1994</v>
+      </c>
+      <c r="B207" t="s">
+        <v>65</v>
+      </c>
+      <c r="C207" t="s">
+        <v>66</v>
+      </c>
+      <c r="D207" t="s">
+        <v>35</v>
+      </c>
+      <c r="E207" t="s">
+        <v>9</v>
+      </c>
+      <c r="F207" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>1994</v>
+      </c>
+      <c r="B208" t="s">
+        <v>48</v>
+      </c>
+      <c r="C208" t="s">
+        <v>49</v>
+      </c>
+      <c r="D208" t="s">
+        <v>35</v>
+      </c>
+      <c r="E208" t="s">
+        <v>37</v>
+      </c>
+      <c r="F208" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>1994</v>
+      </c>
+      <c r="B209" t="s">
+        <v>63</v>
+      </c>
+      <c r="C209" t="s">
+        <v>32</v>
+      </c>
+      <c r="D209" t="s">
+        <v>35</v>
+      </c>
+      <c r="E209" t="s">
+        <v>56</v>
+      </c>
+      <c r="F209" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>1994</v>
+      </c>
+      <c r="B210" t="s">
+        <v>39</v>
+      </c>
+      <c r="C210" t="s">
+        <v>70</v>
+      </c>
+      <c r="D210" t="s">
+        <v>35</v>
+      </c>
+      <c r="E210" t="s">
+        <v>69</v>
+      </c>
+      <c r="F210" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>1994</v>
+      </c>
+      <c r="B211" t="s">
+        <v>36</v>
+      </c>
+      <c r="C211" t="s">
+        <v>64</v>
+      </c>
+      <c r="D211" t="s">
+        <v>35</v>
+      </c>
+      <c r="E211" t="s">
+        <v>15</v>
+      </c>
+      <c r="F211" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>1994</v>
+      </c>
+      <c r="B212" t="s">
+        <v>46</v>
+      </c>
+      <c r="C212" t="s">
+        <v>32</v>
+      </c>
+      <c r="D212" t="s">
+        <v>35</v>
+      </c>
+      <c r="E212" t="s">
+        <v>17</v>
+      </c>
+      <c r="F212" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>1994</v>
+      </c>
+      <c r="B213" t="s">
+        <v>61</v>
+      </c>
+      <c r="C213" t="s">
+        <v>62</v>
+      </c>
+      <c r="D213" t="s">
+        <v>35</v>
+      </c>
+      <c r="E213" t="s">
+        <v>19</v>
+      </c>
+      <c r="F213" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>1994</v>
+      </c>
+      <c r="B214" t="s">
+        <v>46</v>
+      </c>
+      <c r="C214" t="s">
+        <v>64</v>
+      </c>
+      <c r="D214" t="s">
+        <v>35</v>
+      </c>
+      <c r="E214" t="s">
+        <v>71</v>
+      </c>
+      <c r="F214" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>1994</v>
+      </c>
+      <c r="B215" t="s">
+        <v>72</v>
+      </c>
+      <c r="C215" t="s">
+        <v>73</v>
+      </c>
+      <c r="D215" t="s">
+        <v>35</v>
+      </c>
+      <c r="E215" t="s">
+        <v>74</v>
+      </c>
+      <c r="F215" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>1993</v>
+      </c>
+      <c r="B216" t="s">
+        <v>65</v>
+      </c>
+      <c r="C216" t="s">
+        <v>66</v>
+      </c>
+      <c r="D216" t="s">
+        <v>35</v>
+      </c>
+      <c r="E216" t="s">
+        <v>37</v>
+      </c>
+      <c r="F216" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>1993</v>
+      </c>
+      <c r="B217" t="s">
+        <v>48</v>
+      </c>
+      <c r="C217" t="s">
+        <v>49</v>
+      </c>
+      <c r="D217" t="s">
+        <v>35</v>
+      </c>
+      <c r="E217" t="s">
+        <v>9</v>
+      </c>
+      <c r="F217" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>1993</v>
+      </c>
+      <c r="B218" t="s">
+        <v>63</v>
+      </c>
+      <c r="C218" t="s">
+        <v>32</v>
+      </c>
+      <c r="D218" t="s">
+        <v>35</v>
+      </c>
+      <c r="E218" t="s">
+        <v>56</v>
+      </c>
+      <c r="F218" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>1993</v>
+      </c>
+      <c r="B219" t="s">
+        <v>39</v>
+      </c>
+      <c r="C219" t="s">
+        <v>70</v>
+      </c>
+      <c r="D219" t="s">
+        <v>35</v>
+      </c>
+      <c r="E219" t="s">
+        <v>69</v>
+      </c>
+      <c r="F219" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>1993</v>
+      </c>
+      <c r="B220" t="s">
+        <v>36</v>
+      </c>
+      <c r="C220" t="s">
+        <v>64</v>
+      </c>
+      <c r="D220" t="s">
+        <v>35</v>
+      </c>
+      <c r="E220" t="s">
+        <v>15</v>
+      </c>
+      <c r="F220" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>1993</v>
+      </c>
+      <c r="B221" t="s">
+        <v>46</v>
+      </c>
+      <c r="C221" t="s">
+        <v>32</v>
+      </c>
+      <c r="D221" t="s">
+        <v>35</v>
+      </c>
+      <c r="E221" t="s">
+        <v>17</v>
+      </c>
+      <c r="F221" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>1993</v>
+      </c>
+      <c r="B222" t="s">
+        <v>61</v>
+      </c>
+      <c r="C222" t="s">
+        <v>62</v>
+      </c>
+      <c r="D222" t="s">
+        <v>35</v>
+      </c>
+      <c r="E222" t="s">
+        <v>19</v>
+      </c>
+      <c r="F222" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>1993</v>
+      </c>
+      <c r="B223" t="s">
+        <v>46</v>
+      </c>
+      <c r="C223" t="s">
+        <v>64</v>
+      </c>
+      <c r="D223" t="s">
+        <v>35</v>
+      </c>
+      <c r="E223" t="s">
+        <v>71</v>
+      </c>
+      <c r="F223" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>1993</v>
+      </c>
+      <c r="B224" t="s">
+        <v>72</v>
+      </c>
+      <c r="C224" t="s">
+        <v>73</v>
+      </c>
+      <c r="D224" t="s">
+        <v>35</v>
+      </c>
+      <c r="E224" t="s">
+        <v>74</v>
+      </c>
+      <c r="F224" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>